<commit_message>
Fix model sheet -- 'type' now looks to match the prompt type and expands recursively.
</commit_message>
<xml_diff>
--- a/form-files/tables/refrigerators/forms/refrigerators_init/refrigerators_init.xlsx
+++ b/form-files/tables/refrigerators/forms/refrigerators_init/refrigerators_init.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>type</t>
   </si>
@@ -84,15 +84,6 @@
     <t>Terrible</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>object</t>
-  </si>
-  <si>
     <t>refrigerator_stock_level</t>
   </si>
   <si>
@@ -127,9 +118,6 @@
   </si>
   <si>
     <t>survey</t>
-  </si>
-  <si>
-    <t>elementType</t>
   </si>
   <si>
     <t>choice_list_name</t>
@@ -524,19 +512,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -568,7 +556,7 @@
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -614,13 +602,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -690,71 +678,64 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.453125" customWidth="1"/>
     <col min="2" max="2" width="25.1796875" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -784,34 +765,34 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1">
         <v>20130408</v>
@@ -819,10 +800,10 @@
     </row>
     <row r="5" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Display a popup showing when the model is incorrect and the user tries to create a new instance.
</commit_message>
<xml_diff>
--- a/form-files/tables/refrigerators/forms/refrigerators_init/refrigerators_init.xlsx
+++ b/form-files/tables/refrigerators/forms/refrigerators_init/refrigerators_init.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="6040" yWindow="460" windowWidth="25460" windowHeight="10660" activeTab="2"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>type</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>hideInContents</t>
+  </si>
+  <si>
+    <t>refrigerator_text</t>
   </si>
 </sst>
 </file>
@@ -497,17 +500,17 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="41.81640625" customWidth="1"/>
-    <col min="5" max="5" width="32.81640625" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="4" max="4" width="41.83203125" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +530,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -539,7 +542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="18" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -554,7 +557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -568,7 +571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="18" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -598,9 +601,9 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.25" customHeight="1">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -611,7 +614,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16.25" customHeight="1">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -622,7 +625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16.25" customHeight="1">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -633,7 +636,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16.25" customHeight="1">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -644,7 +647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16.25" customHeight="1">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -655,7 +658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.25" customHeight="1">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -678,19 +681,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="12.75" customHeight="1">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -698,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="12.75" customHeight="1">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -706,7 +709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -714,7 +717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -722,7 +725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -730,12 +733,20 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -756,14 +767,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" customWidth="1"/>
-    <col min="3" max="3" width="28.6328125" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -774,7 +785,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -782,7 +793,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -790,7 +801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -798,7 +809,7 @@
         <v>20130408</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
@@ -806,8 +817,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" ht="16.75" customHeight="1"/>
+    <row r="7" spans="1:3" ht="16.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>